<commit_message>
protocol update, upper app add rx check interfaceaceacece“
</commit_message>
<xml_diff>
--- a/document/通讯协议定义.xlsx
+++ b/document/通讯协议定义.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="242" yWindow="109" windowWidth="14799" windowHeight="8011" activeTab="1"/>
+    <workbookView xWindow="242" yWindow="109" windowWidth="14799" windowHeight="8011"/>
   </bookViews>
   <sheets>
     <sheet name="UART通讯协议相关" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="123">
   <si>
     <t>数据通讯</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(n*1)Byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>起始位(1Byte）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -54,10 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数据区     (n Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>错误校验位         (2 Byte)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -276,30 +268,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数据区            (n Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0~255</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地址位            (1Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据编号(2Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0~65536</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>循环冗余校验(CRC)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>指令(1Byte)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -372,10 +344,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>n          (范围0~1024)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>REG 0x0040</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -476,10 +444,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>打开LED:5a 01 32 23 00 08 02 00 00 00 03 03 00 01 FF FF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>串口信息配置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -489,6 +453,58 @@
   </si>
   <si>
     <t>网络信息配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n(范围0~1024)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机数据编号(2Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加密区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非加密区(加密后数据校验)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非加密区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(n-4)Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据区            (n-4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACK                 (1Byte）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>循环冗余校验(CRC) --不包含起始位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开LED:5a 00 0B 01 32 23 02 00 00 00 03 03 00 01 FF FF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(n-3)Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据区     (n-3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回值 5b 00 04 01 32 23 00 ff ff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -695,11 +711,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -740,6 +767,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -764,6 +812,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -782,35 +839,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1113,29 +1143,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.77734375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="13.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1145,257 +1176,295 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="43.6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="38.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.05" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="29.05" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="B12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C12" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="20.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C13" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>56</v>
+      <c r="F22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="25.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="C14:D14"/>
+  <mergeCells count="12">
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,288 +1476,288 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.21875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="28"/>
-    <col min="4" max="4" width="21.5546875" style="28" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="28" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="28" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="28" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="28"/>
+    <col min="1" max="2" width="18.21875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="14"/>
+    <col min="4" max="4" width="21.5546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B3" s="14" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
+      <c r="A5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17">
         <v>7</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="17">
         <v>6</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="17">
         <v>5</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="17">
         <v>4</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="18">
         <v>3</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="17">
         <v>2</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="17">
         <v>1</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="37" t="s">
+      <c r="A7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="56.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="56.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>42</v>
+      <c r="H8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
+      <c r="A10" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17">
         <v>7</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="17">
         <v>6</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="17">
         <v>5</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="17">
         <v>4</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="17">
         <v>3</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="17">
         <v>2</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="17">
         <v>1</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
+      <c r="A16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
     </row>
     <row r="17" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17">
         <v>7</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="17">
         <v>6</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="17">
         <v>5</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="17">
         <v>4</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="17">
         <v>3</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="17">
         <v>2</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="17">
         <v>1</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="25.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1731,18 +1800,18 @@
     <row r="1" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+        <v>82</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
@@ -1773,57 +1842,57 @@
     </row>
     <row r="4" spans="1:9" s="8" customFormat="1" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="8" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+        <v>88</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
@@ -1854,49 +1923,49 @@
     </row>
     <row r="10" spans="1:9" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
     </row>
     <row r="11" spans="1:9" ht="27.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="13" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="27"/>
+        <v>90</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
@@ -1927,47 +1996,47 @@
     </row>
     <row r="16" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="19" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
+        <v>91</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
     </row>
     <row r="21" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
@@ -1998,47 +2067,47 @@
     </row>
     <row r="22" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="34"/>
     </row>
     <row r="25" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
     </row>
     <row r="27" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
@@ -2069,48 +2138,48 @@
     </row>
     <row r="28" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="34"/>
     </row>
     <row r="29" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="34"/>
     </row>
     <row r="30" spans="1:9" ht="11.95" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="31" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
+        <v>87</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
     </row>
     <row r="33" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
@@ -2141,49 +2210,49 @@
     </row>
     <row r="34" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="34"/>
     </row>
     <row r="35" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="34"/>
     </row>
     <row r="37" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="27"/>
+        <v>95</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="37"/>
     </row>
     <row r="39" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
@@ -2214,29 +2283,29 @@
     </row>
     <row r="40" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
     </row>
     <row r="41" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="34"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B42" s="12"/>
@@ -2251,18 +2320,18 @@
     <row r="43" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="27"/>
+        <v>96</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
     </row>
     <row r="45" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
@@ -2293,29 +2362,29 @@
     </row>
     <row r="46" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="34"/>
     </row>
     <row r="47" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B47" s="32"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="34"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B48" s="12"/>
@@ -2330,18 +2399,18 @@
     <row r="49" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="27"/>
+        <v>97</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="37"/>
     </row>
     <row r="51" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
@@ -2372,45 +2441,45 @@
     </row>
     <row r="52" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B52" s="32"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="34"/>
     </row>
     <row r="53" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B53" s="32"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="34"/>
     </row>
     <row r="55" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="27"/>
+        <v>98</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="37"/>
     </row>
     <row r="57" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11"/>
@@ -2441,45 +2510,45 @@
     </row>
     <row r="58" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="22"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B58" s="32"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
     </row>
     <row r="59" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B59" s="32"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="34"/>
     </row>
     <row r="61" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="27"/>
+        <v>99</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="37"/>
     </row>
     <row r="63" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11"/>
@@ -2510,45 +2579,45 @@
     </row>
     <row r="64" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B64" s="32"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="34"/>
     </row>
     <row r="65" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
-      <c r="H65" s="23"/>
-      <c r="I65" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B65" s="32"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="34"/>
     </row>
     <row r="67" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="68" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B68" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="26"/>
-      <c r="G68" s="26"/>
-      <c r="H68" s="26"/>
-      <c r="I68" s="27"/>
+        <v>100</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="37"/>
     </row>
     <row r="69" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11"/>
@@ -2579,45 +2648,45 @@
     </row>
     <row r="70" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="23"/>
-      <c r="H70" s="23"/>
-      <c r="I70" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B70" s="32"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="34"/>
     </row>
     <row r="71" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B71" s="22"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="23"/>
-      <c r="H71" s="23"/>
-      <c r="I71" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B71" s="32"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="33"/>
+      <c r="I71" s="34"/>
     </row>
     <row r="73" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="26"/>
-      <c r="H74" s="26"/>
-      <c r="I74" s="27"/>
+        <v>101</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="37"/>
     </row>
     <row r="75" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11"/>
@@ -2648,45 +2717,45 @@
     </row>
     <row r="76" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="22"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="23"/>
-      <c r="I76" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B76" s="32"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="34"/>
     </row>
     <row r="77" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" s="22"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
-      <c r="H77" s="23"/>
-      <c r="I77" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B77" s="32"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="33"/>
+      <c r="I77" s="34"/>
     </row>
     <row r="79" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B80" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
-      <c r="E80" s="26"/>
-      <c r="F80" s="26"/>
-      <c r="G80" s="26"/>
-      <c r="H80" s="26"/>
-      <c r="I80" s="27"/>
+        <v>102</v>
+      </c>
+      <c r="B80" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="36"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="36"/>
+      <c r="I80" s="37"/>
     </row>
     <row r="81" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11"/>
@@ -2717,45 +2786,45 @@
     </row>
     <row r="82" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B82" s="32"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="33"/>
+      <c r="I82" s="34"/>
     </row>
     <row r="83" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B83" s="22"/>
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="23"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="23"/>
-      <c r="I83" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B83" s="32"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="34"/>
     </row>
     <row r="85" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="86" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B86" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="26"/>
-      <c r="F86" s="26"/>
-      <c r="G86" s="26"/>
-      <c r="H86" s="26"/>
-      <c r="I86" s="27"/>
+        <v>103</v>
+      </c>
+      <c r="B86" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="36"/>
+      <c r="I86" s="37"/>
     </row>
     <row r="87" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11"/>
@@ -2786,45 +2855,45 @@
     </row>
     <row r="88" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B88" s="22"/>
-      <c r="C88" s="23"/>
-      <c r="D88" s="23"/>
-      <c r="E88" s="23"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="23"/>
-      <c r="H88" s="23"/>
-      <c r="I88" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B88" s="32"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="34"/>
     </row>
     <row r="89" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B89" s="22"/>
-      <c r="C89" s="23"/>
-      <c r="D89" s="23"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="23"/>
-      <c r="H89" s="23"/>
-      <c r="I89" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B89" s="32"/>
+      <c r="C89" s="33"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="33"/>
+      <c r="I89" s="34"/>
     </row>
     <row r="91" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="92" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B92" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="26"/>
-      <c r="H92" s="26"/>
-      <c r="I92" s="27"/>
+        <v>104</v>
+      </c>
+      <c r="B92" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C92" s="36"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="37"/>
     </row>
     <row r="93" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11"/>
@@ -2855,33 +2924,33 @@
     </row>
     <row r="94" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B94" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C94" s="23"/>
-      <c r="D94" s="23"/>
-      <c r="E94" s="23"/>
-      <c r="F94" s="23"/>
-      <c r="G94" s="23"/>
-      <c r="H94" s="23"/>
-      <c r="I94" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="B94" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="33"/>
+      <c r="G94" s="33"/>
+      <c r="H94" s="33"/>
+      <c r="I94" s="34"/>
     </row>
     <row r="95" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B95" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="23"/>
-      <c r="H95" s="23"/>
-      <c r="I95" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B95" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="33"/>
+      <c r="F95" s="33"/>
+      <c r="G95" s="33"/>
+      <c r="H95" s="33"/>
+      <c r="I95" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="48">

</xml_diff>

<commit_message>
file update add, Reduce CPU utilization
</commit_message>
<xml_diff>
--- a/document/通讯协议定义.xlsx
+++ b/document/通讯协议定义.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="242" yWindow="109" windowWidth="14799" windowHeight="8011" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="UART通讯协议相关" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="121">
   <si>
     <t>数据通讯</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -296,10 +296,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上传指令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x04</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,10 +320,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cmd(1)+size(2)+data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cmd(1)+reg(2)+size(2)+data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -493,6 +485,18 @@
   </si>
   <si>
     <t>返回值 5b 00 04 01 32 23 00 ff ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传开始指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd(1)+文件总长度(4)+字符串名称，以0结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd(1)+后续文件长度(2)+data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1133,28 +1137,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="15.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1164,27 +1168,27 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="43.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1198,32 +1202,32 @@
         <v>60</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="38.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="23"/>
       <c r="F6" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29.05" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>61</v>
       </c>
@@ -1236,7 +1240,7 @@
       <c r="D9" s="23"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
@@ -1249,7 +1253,7 @@
       <c r="D10" s="26"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -1257,68 +1261,68 @@
         <v>68</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="20.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C13" s="25" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="23"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
@@ -1329,7 +1333,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -1340,24 +1344,24 @@
         <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>3</v>
@@ -1369,28 +1373,28 @@
         <v>50</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="25.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="25.7" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="23"/>
       <c r="G23" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1398,7 +1402,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1406,7 +1410,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1414,7 +1418,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1430,9 +1434,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -1464,24 +1468,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:I13"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="18.21875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="21.5546875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="14" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="2" width="18.25" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="14"/>
+    <col min="4" max="4" width="21.5" style="14" customWidth="1"/>
+    <col min="5" max="5" width="20.125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="18.25" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.875" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="8.875" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
@@ -1489,7 +1493,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
@@ -1497,8 +1501,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>22</v>
       </c>
@@ -1513,7 +1517,7 @@
       <c r="H5" s="31"/>
       <c r="I5" s="32"/>
     </row>
-    <row r="6" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="17">
         <v>7</v>
@@ -1540,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -1549,13 +1553,13 @@
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>41</v>
@@ -1567,7 +1571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="56.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
@@ -1576,13 +1580,13 @@
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>39</v>
@@ -1594,8 +1598,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>44</v>
       </c>
@@ -1610,7 +1614,7 @@
       <c r="H10" s="31"/>
       <c r="I10" s="32"/>
     </row>
-    <row r="11" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="17">
         <v>7</v>
@@ -1637,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
@@ -1652,7 +1656,7 @@
       <c r="H12" s="28"/>
       <c r="I12" s="29"/>
     </row>
-    <row r="13" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -1665,8 +1669,8 @@
       <c r="H13" s="28"/>
       <c r="I13" s="29"/>
     </row>
-    <row r="15" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
@@ -1681,7 +1685,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="17">
         <v>7</v>
@@ -1708,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="25.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>11</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>12</v>
       </c>
@@ -1772,24 +1776,24 @@
       <selection activeCell="B82" sqref="B82:I82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="18.21875" style="9" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" style="9"/>
-    <col min="6" max="6" width="15.6640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="2" width="18.25" style="9" customWidth="1"/>
+    <col min="3" max="5" width="8.875" style="9"/>
+    <col min="6" max="6" width="15.625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.25" style="9" customWidth="1"/>
+    <col min="9" max="9" width="21.875" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="8.875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>81</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -1799,7 +1803,7 @@
       <c r="H2" s="37"/>
       <c r="I2" s="38"/>
     </row>
-    <row r="3" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="7">
         <v>7</v>
@@ -1826,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="8" customFormat="1" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="8" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -1864,13 +1868,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
@@ -1880,7 +1884,7 @@
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
     </row>
-    <row r="9" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="7">
         <v>7</v>
@@ -1907,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -1922,12 +1926,12 @@
       <c r="H10" s="34"/>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:9" ht="27.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -1937,13 +1941,13 @@
       <c r="H11" s="34"/>
       <c r="I11" s="35"/>
     </row>
-    <row r="13" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -1953,7 +1957,7 @@
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="7">
         <v>7</v>
@@ -1980,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
@@ -1995,7 +1999,7 @@
       <c r="H16" s="34"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>12</v>
       </c>
@@ -2008,13 +2012,13 @@
       <c r="H17" s="34"/>
       <c r="I17" s="35"/>
     </row>
-    <row r="19" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
@@ -2024,7 +2028,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="7">
         <v>7</v>
@@ -2051,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
@@ -2066,7 +2070,7 @@
       <c r="H22" s="34"/>
       <c r="I22" s="35"/>
     </row>
-    <row r="23" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -2079,13 +2083,13 @@
       <c r="H23" s="34"/>
       <c r="I23" s="35"/>
     </row>
-    <row r="25" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
@@ -2095,7 +2099,7 @@
       <c r="H26" s="37"/>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="7">
         <v>7</v>
@@ -2122,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2141,7 @@
       <c r="H28" s="34"/>
       <c r="I28" s="35"/>
     </row>
-    <row r="29" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2150,14 +2154,14 @@
       <c r="H29" s="34"/>
       <c r="I29" s="35"/>
     </row>
-    <row r="30" spans="1:9" ht="11.95" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
@@ -2167,7 +2171,7 @@
       <c r="H32" s="37"/>
       <c r="I32" s="38"/>
     </row>
-    <row r="33" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="7">
         <v>7</v>
@@ -2194,12 +2198,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C34" s="34"/>
       <c r="D34" s="34"/>
@@ -2209,7 +2213,7 @@
       <c r="H34" s="34"/>
       <c r="I34" s="35"/>
     </row>
-    <row r="35" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -2224,13 +2228,13 @@
       <c r="H35" s="34"/>
       <c r="I35" s="35"/>
     </row>
-    <row r="37" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
@@ -2240,7 +2244,7 @@
       <c r="H38" s="37"/>
       <c r="I38" s="38"/>
     </row>
-    <row r="39" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="7">
         <v>7</v>
@@ -2267,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>11</v>
       </c>
@@ -2280,7 +2284,7 @@
       <c r="H40" s="34"/>
       <c r="I40" s="35"/>
     </row>
-    <row r="41" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>12</v>
       </c>
@@ -2303,10 +2307,10 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B44" s="36" t="s">
         <v>16</v>
@@ -2319,7 +2323,7 @@
       <c r="H44" s="37"/>
       <c r="I44" s="38"/>
     </row>
-    <row r="45" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="7">
         <v>7</v>
@@ -2346,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>11</v>
       </c>
@@ -2359,7 +2363,7 @@
       <c r="H46" s="34"/>
       <c r="I46" s="35"/>
     </row>
-    <row r="47" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>12</v>
       </c>
@@ -2382,10 +2386,10 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B50" s="36" t="s">
         <v>17</v>
@@ -2398,7 +2402,7 @@
       <c r="H50" s="37"/>
       <c r="I50" s="38"/>
     </row>
-    <row r="51" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
       <c r="B51" s="7">
         <v>7</v>
@@ -2425,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>11</v>
       </c>
@@ -2438,7 +2442,7 @@
       <c r="H52" s="34"/>
       <c r="I52" s="35"/>
     </row>
-    <row r="53" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>12</v>
       </c>
@@ -2451,10 +2455,10 @@
       <c r="H53" s="34"/>
       <c r="I53" s="35"/>
     </row>
-    <row r="55" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B56" s="36" t="s">
         <v>27</v>
@@ -2467,7 +2471,7 @@
       <c r="H56" s="37"/>
       <c r="I56" s="38"/>
     </row>
-    <row r="57" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11"/>
       <c r="B57" s="7">
         <v>7</v>
@@ -2494,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>11</v>
       </c>
@@ -2507,7 +2511,7 @@
       <c r="H58" s="34"/>
       <c r="I58" s="35"/>
     </row>
-    <row r="59" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>12</v>
       </c>
@@ -2520,10 +2524,10 @@
       <c r="H59" s="34"/>
       <c r="I59" s="35"/>
     </row>
-    <row r="61" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B62" s="36" t="s">
         <v>28</v>
@@ -2536,7 +2540,7 @@
       <c r="H62" s="37"/>
       <c r="I62" s="38"/>
     </row>
-    <row r="63" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11"/>
       <c r="B63" s="7">
         <v>7</v>
@@ -2563,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>11</v>
       </c>
@@ -2576,7 +2580,7 @@
       <c r="H64" s="34"/>
       <c r="I64" s="35"/>
     </row>
-    <row r="65" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>12</v>
       </c>
@@ -2589,10 +2593,10 @@
       <c r="H65" s="34"/>
       <c r="I65" s="35"/>
     </row>
-    <row r="67" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B68" s="36" t="s">
         <v>29</v>
@@ -2605,7 +2609,7 @@
       <c r="H68" s="37"/>
       <c r="I68" s="38"/>
     </row>
-    <row r="69" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11"/>
       <c r="B69" s="7">
         <v>7</v>
@@ -2632,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>11</v>
       </c>
@@ -2645,7 +2649,7 @@
       <c r="H70" s="34"/>
       <c r="I70" s="35"/>
     </row>
-    <row r="71" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>12</v>
       </c>
@@ -2658,10 +2662,10 @@
       <c r="H71" s="34"/>
       <c r="I71" s="35"/>
     </row>
-    <row r="73" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B74" s="36" t="s">
         <v>23</v>
@@ -2674,7 +2678,7 @@
       <c r="H74" s="37"/>
       <c r="I74" s="38"/>
     </row>
-    <row r="75" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11"/>
       <c r="B75" s="7">
         <v>7</v>
@@ -2701,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
         <v>11</v>
       </c>
@@ -2714,7 +2718,7 @@
       <c r="H76" s="34"/>
       <c r="I76" s="35"/>
     </row>
-    <row r="77" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>12</v>
       </c>
@@ -2727,13 +2731,13 @@
       <c r="H77" s="34"/>
       <c r="I77" s="35"/>
     </row>
-    <row r="79" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B80" s="36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="37"/>
@@ -2743,7 +2747,7 @@
       <c r="H80" s="37"/>
       <c r="I80" s="38"/>
     </row>
-    <row r="81" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11"/>
       <c r="B81" s="7">
         <v>7</v>
@@ -2770,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
         <v>11</v>
       </c>
@@ -2783,7 +2787,7 @@
       <c r="H82" s="34"/>
       <c r="I82" s="35"/>
     </row>
-    <row r="83" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>12</v>
       </c>
@@ -2798,25 +2802,16 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B62:I62"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="B70:I70"/>
+    <mergeCell ref="B68:I68"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B77:I77"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="B71:I71"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
@@ -2830,16 +2825,25 @@
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B68:I68"/>
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B77:I77"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B71:I71"/>
+    <mergeCell ref="B62:I62"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B14:I14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lower and upper app update, document update
</commit_message>
<xml_diff>
--- a/document/通讯协议定义.xlsx
+++ b/document/通讯协议定义.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UART通讯协议相关" sheetId="1" r:id="rId1"/>
@@ -472,14 +472,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REG 0x0068~0x006F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RTC内部计数-second(8Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>打开LED:5a 00 0B 01 32 23 02 00 00 00 03 03 00 01 FF FF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -497,6 +489,14 @@
   </si>
   <si>
     <t>cmd(1)+后续文件长度(2)+data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTC内部计数-hour, minute, sec(12Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0068~0x0073</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1137,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:D13"/>
     </sheetView>
   </sheetViews>
@@ -1271,10 +1271,10 @@
         <v>69</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="6"/>
@@ -1287,7 +1287,7 @@
         <v>71</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="6"/>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -1772,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:I82"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2734,10 +2734,10 @@
     <row r="79" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B80" s="36" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="37"/>
@@ -2802,16 +2802,22 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B68:I68"/>
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B77:I77"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B71:I71"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B62:I62"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B59:I59"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
@@ -2825,25 +2831,19 @@
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B62:I62"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B59:I59"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="B70:I70"/>
+    <mergeCell ref="B68:I68"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B77:I77"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="B71:I71"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update for document and system structure.
</commit_message>
<xml_diff>
--- a/document/通讯协议定义.xlsx
+++ b/document/通讯协议定义.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2DCD9C-7112-4D1B-B9D8-394ABA0BCFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UART通讯协议相关" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
   <si>
     <t>数据通讯</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,317 +205,319 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0x5B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACK(1Byte）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应答状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无效指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0~65536</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指令(1Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读内部状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd(1)+reg(2)+size(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写内部状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>示例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据长度   (2Byte，高位在前)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd(1)+reg(2)+size(2)+data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0040</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO模块管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0048~0x0049</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x004A~0x004B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0041~0x0043</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0044~0x0045</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0046~0x0047</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光传感器模块(als数据 2Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红外LED距离(ia数据 2Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接近距离传感器(ps数据 2Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x004C~0x004F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0050~0x0053</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0054~0x0057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0058~0x005B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x005C~0x005F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0060~0x0063</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>软件复位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:软件复位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>串口信息配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0:执行设置完毕               1:执行设置 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络信息配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n(范围0~1024)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机数据编号(2Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加密区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非加密区(加密后数据校验)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非加密区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(n-4)Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据区            (n-4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACK                 (1Byte）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>循环冗余校验(CRC) --不包含起始位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(n-3)Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据区     (n-3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>六轴传感器角速度值(gyro_x数据 4Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0064~0x0067</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开LED:5a 00 0B 01 32 23 02 00 00 00 03 03 00 01 FF FF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回值 5b 00 04 01 32 23 00 ff ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传开始指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd(1)+文件总长度(4)+字符串名称，以0结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd(1)+后续文件长度(2)+data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTC内部计数-hour, minute, sec(12Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG 0x0068~0x0073</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>上位机返回数据结构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x5B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACK(1Byte）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应答状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据正常</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无效指令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xFF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0~65536</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指令(1Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>读内部状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cmd(1)+reg(2)+size(2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>写内部状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>示例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据长度   (2Byte，高位在前)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cmd(1)+reg(2)+size(2)+data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0040</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPIO模块管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0048~0x0049</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x004A~0x004B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0041~0x0043</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0044~0x0045</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0046~0x0047</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>光传感器模块(als数据 2Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红外LED距离(ia数据 2Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接近距离传感器(ps数据 2Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x004C~0x004F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0050~0x0053</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0054~0x0057</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0058~0x005B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x005C~0x005F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0060~0x0063</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>软件复位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1:软件复位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>串口信息配置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0:执行设置完毕               1:执行设置 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络信息配置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n(范围0~1024)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机数据编号(2Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>加密区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>非加密区(加密后数据校验)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>非加密区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(n-4)Byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据区            (n-4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACK                 (1Byte）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>循环冗余校验(CRC) --不包含起始位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(n-3)Byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据区     (n-3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>六轴传感器角速度值(gyro_x数据 4Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0064~0x0067</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开LED:5a 00 0B 01 32 23 02 00 00 00 03 03 00 01 FF FF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回值 5b 00 04 01 32 23 00 ff ff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传开始指令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cmd(1)+文件总长度(4)+字符串名称，以0结束</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cmd(1)+后续文件长度(2)+data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RTC内部计数-hour, minute, sec(12Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG 0x0068~0x0073</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上位机和下位机具有相同的数据结构</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -537,7 +540,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -552,7 +555,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -816,6 +819,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -825,18 +837,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -844,12 +847,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -891,7 +897,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -924,9 +930,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -959,6 +982,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,31 +1174,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" style="2" customWidth="1"/>
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="6" max="6" width="15.08984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1168,27 +1208,27 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="29">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="43.5">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1199,132 +1239,132 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="38.15" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="23"/>
       <c r="F6" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="14.65" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="25" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>66</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="14.65" customHeight="1">
       <c r="A11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="C11" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="27.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>117</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="20.9" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C13" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="14.65" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="23"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" s="5" customFormat="1">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1333,7 +1373,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="29">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -1344,104 +1384,109 @@
         <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="29">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="25.7" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="25.75" customHeight="1">
       <c r="A23" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="23"/>
       <c r="G23" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
+    </row>
+    <row r="35" spans="1:1" ht="29">
+      <c r="A35" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1465,27 +1510,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="18.25" style="14" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="14"/>
-    <col min="4" max="4" width="21.5" style="14" customWidth="1"/>
-    <col min="5" max="5" width="20.125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="18.25" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.875" style="14" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="14"/>
+    <col min="1" max="2" width="18.26953125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="14"/>
+    <col min="4" max="4" width="21.453125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
@@ -1493,7 +1538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
@@ -1501,8 +1546,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" thickBot="1"/>
+    <row r="5" spans="1:9" ht="15.5" thickBot="1">
       <c r="A5" s="15" t="s">
         <v>22</v>
       </c>
@@ -1517,7 +1562,7 @@
       <c r="H5" s="31"/>
       <c r="I5" s="32"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.5" thickBot="1">
       <c r="A6" s="16"/>
       <c r="B6" s="17">
         <v>7</v>
@@ -1544,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.5" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -1553,13 +1598,13 @@
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>41</v>
@@ -1571,7 +1616,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="56.25" customHeight="1" thickBot="1">
       <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
@@ -1580,13 +1625,13 @@
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>39</v>
@@ -1598,8 +1643,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" thickBot="1"/>
+    <row r="10" spans="1:9" ht="15.5" thickBot="1">
       <c r="A10" s="15" t="s">
         <v>44</v>
       </c>
@@ -1614,7 +1659,7 @@
       <c r="H10" s="31"/>
       <c r="I10" s="32"/>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.5" thickBot="1">
       <c r="A11" s="16"/>
       <c r="B11" s="17">
         <v>7</v>
@@ -1641,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.5" thickBot="1">
       <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
@@ -1656,7 +1701,7 @@
       <c r="H12" s="28"/>
       <c r="I12" s="29"/>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.5" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -1669,8 +1714,8 @@
       <c r="H13" s="28"/>
       <c r="I13" s="29"/>
     </row>
-    <row r="15" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" thickBot="1"/>
+    <row r="16" spans="1:9" ht="15.5" thickBot="1">
       <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
@@ -1685,7 +1730,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15.5" thickBot="1">
       <c r="A17" s="16"/>
       <c r="B17" s="17">
         <v>7</v>
@@ -1712,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="25.75" customHeight="1" thickBot="1">
       <c r="A18" s="19" t="s">
         <v>11</v>
       </c>
@@ -1731,7 +1776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1">
       <c r="A19" s="19" t="s">
         <v>12</v>
       </c>
@@ -1769,41 +1814,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="18.25" style="9" customWidth="1"/>
-    <col min="3" max="5" width="8.875" style="9"/>
-    <col min="6" max="6" width="15.625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="18.25" style="9" customWidth="1"/>
-    <col min="9" max="9" width="21.875" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="9"/>
+    <col min="1" max="2" width="18.26953125" style="9" customWidth="1"/>
+    <col min="3" max="5" width="8.90625" style="9"/>
+    <col min="6" max="6" width="15.6328125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="13.5" customHeight="1" thickBot="1"/>
+    <row r="2" spans="1:9" ht="13.5" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38"/>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35"/>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" thickBot="1">
       <c r="A3" s="11"/>
       <c r="B3" s="7">
         <v>7</v>
@@ -1830,18 +1875,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="8" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="8" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="13" t="s">
         <v>36</v>
       </c>
@@ -1849,18 +1894,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="7" t="s">
         <v>33</v>
       </c>
@@ -1868,23 +1913,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="8" spans="1:9" ht="13.5" thickBot="1">
       <c r="A8" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
-    </row>
-    <row r="9" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.5" thickBot="1">
       <c r="A9" s="11"/>
       <c r="B9" s="7">
         <v>7</v>
@@ -1911,53 +1956,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="1:9" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="1:9" ht="27.25" customHeight="1" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+    </row>
+    <row r="13" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="14" spans="1:9" ht="13.5" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.5" thickBot="1">
       <c r="A15" s="11"/>
       <c r="B15" s="7">
         <v>7</v>
@@ -1984,51 +2029,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="13.5" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.5" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="20" spans="1:9" ht="13.5" thickBot="1">
       <c r="A20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.5" thickBot="1">
       <c r="A21" s="11"/>
       <c r="B21" s="7">
         <v>7</v>
@@ -2055,51 +2100,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12" customHeight="1" thickBot="1">
       <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="35"/>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" thickBot="1">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="35"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="26" spans="1:9" ht="13.5" thickBot="1">
       <c r="A26" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.5" thickBot="1">
       <c r="A27" s="11"/>
       <c r="B27" s="7">
         <v>7</v>
@@ -2126,52 +2171,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="13.5" thickBot="1">
       <c r="A28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="35"/>
-    </row>
-    <row r="29" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="38"/>
+    </row>
+    <row r="29" spans="1:9" ht="12" customHeight="1" thickBot="1">
       <c r="A29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="35"/>
-    </row>
-    <row r="30" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+    </row>
+    <row r="30" spans="1:9" ht="12" customHeight="1"/>
+    <row r="31" spans="1:9" ht="12" customHeight="1" thickBot="1"/>
+    <row r="32" spans="1:9" ht="13.5" thickBot="1">
       <c r="A32" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
-    </row>
-    <row r="33" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="35"/>
+    </row>
+    <row r="33" spans="1:9" ht="13.5" thickBot="1">
       <c r="A33" s="11"/>
       <c r="B33" s="7">
         <v>7</v>
@@ -2198,53 +2243,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="13.5" thickBot="1">
       <c r="A34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="35"/>
-    </row>
-    <row r="35" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="38"/>
+    </row>
+    <row r="35" spans="1:9" ht="13.5" thickBot="1">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="35"/>
-    </row>
-    <row r="37" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="38"/>
+    </row>
+    <row r="37" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="38" spans="1:9" ht="13.5" thickBot="1">
       <c r="A38" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="35"/>
+    </row>
+    <row r="39" spans="1:9" ht="13.5" thickBot="1">
       <c r="A39" s="11"/>
       <c r="B39" s="7">
         <v>7</v>
@@ -2271,33 +2316,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="13.5" thickBot="1">
       <c r="A40" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="35"/>
-    </row>
-    <row r="41" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+    </row>
+    <row r="41" spans="1:9" ht="13.5" thickBot="1">
       <c r="A41" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="35"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
+    </row>
+    <row r="42" spans="1:9">
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -2307,23 +2352,23 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="44" spans="1:9" ht="13.5" thickBot="1">
       <c r="A44" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
-    </row>
-    <row r="45" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="35"/>
+    </row>
+    <row r="45" spans="1:9" ht="13.5" thickBot="1">
       <c r="A45" s="11"/>
       <c r="B45" s="7">
         <v>7</v>
@@ -2350,33 +2395,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="13.5" thickBot="1">
       <c r="A46" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="35"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="1:9" ht="13.5" thickBot="1">
       <c r="A47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="35"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B47" s="36"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
+    </row>
+    <row r="48" spans="1:9">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -2386,23 +2431,23 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="50" spans="1:9" ht="13.5" thickBot="1">
       <c r="A50" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
-    </row>
-    <row r="51" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="35"/>
+    </row>
+    <row r="51" spans="1:9" ht="13.5" thickBot="1">
       <c r="A51" s="11"/>
       <c r="B51" s="7">
         <v>7</v>
@@ -2429,49 +2474,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="13.5" thickBot="1">
       <c r="A52" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="35"/>
-    </row>
-    <row r="53" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="38"/>
+    </row>
+    <row r="53" spans="1:9" ht="13.5" thickBot="1">
       <c r="A53" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="35"/>
-    </row>
-    <row r="55" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="36"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="38"/>
+    </row>
+    <row r="55" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="56" spans="1:9" ht="13.5" thickBot="1">
       <c r="A56" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="38"/>
-    </row>
-    <row r="57" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="35"/>
+    </row>
+    <row r="57" spans="1:9" ht="13.5" thickBot="1">
       <c r="A57" s="11"/>
       <c r="B57" s="7">
         <v>7</v>
@@ -2498,49 +2543,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="13.5" thickBot="1">
       <c r="A58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="35"/>
-    </row>
-    <row r="59" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="36"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="38"/>
+    </row>
+    <row r="59" spans="1:9" ht="13.5" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="35"/>
-    </row>
-    <row r="61" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="36"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="38"/>
+    </row>
+    <row r="61" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="62" spans="1:9" ht="13.5" thickBot="1">
       <c r="A62" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="38"/>
-    </row>
-    <row r="63" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="35"/>
+    </row>
+    <row r="63" spans="1:9" ht="13.5" thickBot="1">
       <c r="A63" s="11"/>
       <c r="B63" s="7">
         <v>7</v>
@@ -2567,49 +2612,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="13.5" thickBot="1">
       <c r="A64" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="33"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="34"/>
-      <c r="H64" s="34"/>
-      <c r="I64" s="35"/>
-    </row>
-    <row r="65" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="36"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="38"/>
+    </row>
+    <row r="65" spans="1:9" ht="13.5" thickBot="1">
       <c r="A65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B65" s="33"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="34"/>
-      <c r="I65" s="35"/>
-    </row>
-    <row r="67" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="36"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="38"/>
+    </row>
+    <row r="67" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="68" spans="1:9" ht="13.5" thickBot="1">
       <c r="A68" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
-      <c r="I68" s="38"/>
-    </row>
-    <row r="69" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="35"/>
+    </row>
+    <row r="69" spans="1:9" ht="13.5" thickBot="1">
       <c r="A69" s="11"/>
       <c r="B69" s="7">
         <v>7</v>
@@ -2636,49 +2681,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="13.5" thickBot="1">
       <c r="A70" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="34"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="35"/>
-    </row>
-    <row r="71" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="36"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="38"/>
+    </row>
+    <row r="71" spans="1:9" ht="13.5" thickBot="1">
       <c r="A71" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="35"/>
-    </row>
-    <row r="73" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="36"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="38"/>
+    </row>
+    <row r="73" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="74" spans="1:9" ht="13.5" thickBot="1">
       <c r="A74" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B74" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="37"/>
-      <c r="H74" s="37"/>
-      <c r="I74" s="38"/>
-    </row>
-    <row r="75" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
+      <c r="H74" s="34"/>
+      <c r="I74" s="35"/>
+    </row>
+    <row r="75" spans="1:9" ht="13.5" thickBot="1">
       <c r="A75" s="11"/>
       <c r="B75" s="7">
         <v>7</v>
@@ -2705,49 +2750,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="13.5" thickBot="1">
       <c r="A76" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
-      <c r="F76" s="34"/>
-      <c r="G76" s="34"/>
-      <c r="H76" s="34"/>
-      <c r="I76" s="35"/>
-    </row>
-    <row r="77" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="36"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="38"/>
+    </row>
+    <row r="77" spans="1:9" ht="13.5" thickBot="1">
       <c r="A77" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="34"/>
-      <c r="H77" s="34"/>
-      <c r="I77" s="35"/>
-    </row>
-    <row r="79" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="36"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="38"/>
+    </row>
+    <row r="79" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="80" spans="1:9" ht="13.5" thickBot="1">
       <c r="A80" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B80" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="37"/>
-      <c r="H80" s="37"/>
-      <c r="I80" s="38"/>
-    </row>
-    <row r="81" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="35"/>
+    </row>
+    <row r="81" spans="1:9" ht="13.5" thickBot="1">
       <c r="A81" s="11"/>
       <c r="B81" s="7">
         <v>7</v>
@@ -2774,50 +2819,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="13.5" thickBot="1">
       <c r="A82" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B82" s="33"/>
-      <c r="C82" s="34"/>
-      <c r="D82" s="34"/>
-      <c r="E82" s="34"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="34"/>
-      <c r="H82" s="34"/>
-      <c r="I82" s="35"/>
-    </row>
-    <row r="83" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="36"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="38"/>
+    </row>
+    <row r="83" spans="1:9" ht="13.5" thickBot="1">
       <c r="A83" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="33"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="34"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="35"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B62:I62"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="B70:I70"/>
+    <mergeCell ref="B68:I68"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B77:I77"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="B71:I71"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
@@ -2834,16 +2873,22 @@
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B68:I68"/>
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B77:I77"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B71:I71"/>
+    <mergeCell ref="B62:I62"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B14:I14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support for protocol update and config save.
</commit_message>
<xml_diff>
--- a/document/通讯协议定义.xlsx
+++ b/document/通讯协议定义.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2DCD9C-7112-4D1B-B9D8-394ABA0BCFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426E33A2-90C8-4717-B677-F8E17EF33CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,12 +12,25 @@
     <sheet name="配置寄存器" sheetId="2" r:id="rId2"/>
     <sheet name="状态寄存器" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="141">
   <si>
     <t>数据通讯</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -501,6 +514,63 @@
   </si>
   <si>
     <t>上位机和下位机具有相同的数据结构</t>
+  </si>
+  <si>
+    <t>通讯为异步</t>
+  </si>
+  <si>
+    <t>数据结构</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>2Byte</t>
+  </si>
+  <si>
+    <t>序列号</t>
+  </si>
+  <si>
+    <t>1Byte</t>
+  </si>
+  <si>
+    <t>包类型</t>
+  </si>
+  <si>
+    <t>包类型-SID</t>
+  </si>
+  <si>
+    <t>4bit-4bit</t>
+  </si>
+  <si>
+    <t>DataLength</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>nByte</t>
+  </si>
+  <si>
+    <t>CRC16</t>
+  </si>
+  <si>
+    <t>SYN</t>
+  </si>
+  <si>
+    <t>bit7</t>
+  </si>
+  <si>
+    <t>ACK</t>
+  </si>
+  <si>
+    <t>bit6</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>bit0~bit3</t>
   </si>
 </sst>
 </file>
@@ -819,6 +889,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -826,15 +905,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1175,15 +1245,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.08984375" style="2" customWidth="1"/>
@@ -1195,313 +1265,398 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1">
-      <c r="A3" s="3" t="s">
+    <row r="42" spans="1:6" s="5" customFormat="1">
+      <c r="A42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="29">
-      <c r="A4" s="3" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" s="5" customFormat="1" ht="29">
+      <c r="A43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="43.5">
-      <c r="A5" s="3" t="s">
+    <row r="44" spans="1:6" s="5" customFormat="1" ht="43.5">
+      <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="38.15" customHeight="1">
-      <c r="A6" s="22" t="s">
+    <row r="45" spans="1:6" s="5" customFormat="1" ht="38.15" customHeight="1">
+      <c r="A45" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24" t="s">
+      <c r="B45" s="23"/>
+      <c r="C45" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="3" t="s">
+      <c r="D45" s="24"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29">
-      <c r="A8" s="2" t="s">
+    <row r="47" spans="1:6" ht="29">
+      <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C48" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.65" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="D48" s="23"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" ht="14.65" customHeight="1">
+      <c r="A49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C49" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.65" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="D49" s="26"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" ht="14.65" customHeight="1">
+      <c r="A50" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C50" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="D50" s="26"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A51" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C51" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="20.9" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="D51" s="26"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" ht="20.9" customHeight="1">
+      <c r="A52" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C52" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.65" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3" t="s">
+      <c r="D52" s="26"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" ht="14.65" customHeight="1">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="21" t="s">
+    <row r="57" spans="1:7">
+      <c r="A57" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-    </row>
-    <row r="20" spans="1:7" s="5" customFormat="1">
-      <c r="A20" s="3" t="s">
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+    </row>
+    <row r="59" spans="1:7" s="5" customFormat="1">
+      <c r="A59" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="29">
-      <c r="A21" s="3" t="s">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" s="5" customFormat="1" ht="29">
+      <c r="A60" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F60" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="29">
-      <c r="A22" s="3" t="s">
+    <row r="61" spans="1:7" s="5" customFormat="1" ht="29">
+      <c r="A61" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="25.75" customHeight="1">
-      <c r="A23" s="22" t="s">
+    <row r="62" spans="1:7" ht="25.75" customHeight="1">
+      <c r="A62" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="22" t="s">
+      <c r="B62" s="23"/>
+      <c r="C62" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="3" t="s">
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
+    <row r="64" spans="1:7">
+      <c r="A64" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
+    <row r="65" spans="1:5">
+      <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
+    <row r="66" spans="1:5">
+      <c r="A66" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
+    <row r="67" spans="1:5">
+      <c r="A67" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
+    <row r="68" spans="1:5">
+      <c r="A68" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="21" t="s">
+    <row r="70" spans="1:5">
+      <c r="A70" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="35" spans="1:1" ht="29">
-      <c r="A35" s="2" t="s">
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="74" spans="1:5" ht="29">
+      <c r="A74" s="2" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1837,16 +1992,16 @@
       <c r="A2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9" ht="13.5" thickBot="1">
       <c r="A3" s="11"/>
@@ -1879,14 +2034,14 @@
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="13" t="s">
         <v>36</v>
       </c>
@@ -1898,14 +2053,14 @@
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="7" t="s">
         <v>33</v>
       </c>
@@ -1918,16 +2073,16 @@
       <c r="A8" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:9" ht="13.5" thickBot="1">
       <c r="A9" s="11"/>
@@ -1960,47 +2115,47 @@
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:9" ht="27.25" customHeight="1" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="13" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="14" spans="1:9" ht="13.5" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="35"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:9" ht="13.5" thickBot="1">
       <c r="A15" s="11"/>
@@ -2033,45 +2188,45 @@
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="35"/>
     </row>
     <row r="17" spans="1:9" ht="13.5" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
     </row>
     <row r="19" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="20" spans="1:9" ht="13.5" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="35"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" thickBot="1">
       <c r="A21" s="11"/>
@@ -2104,45 +2259,45 @@
       <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:9" ht="13.5" thickBot="1">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="35"/>
     </row>
     <row r="25" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="26" spans="1:9" ht="13.5" thickBot="1">
       <c r="A26" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="35"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:9" ht="13.5" thickBot="1">
       <c r="A27" s="11"/>
@@ -2175,29 +2330,29 @@
       <c r="A28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="38"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" ht="12" customHeight="1" thickBot="1">
       <c r="A29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:9" ht="12" customHeight="1"/>
     <row r="31" spans="1:9" ht="12" customHeight="1" thickBot="1"/>
@@ -2205,16 +2360,16 @@
       <c r="A32" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="35"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
     </row>
     <row r="33" spans="1:9" ht="13.5" thickBot="1">
       <c r="A33" s="11"/>
@@ -2247,47 +2402,47 @@
       <c r="A34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="35"/>
     </row>
     <row r="35" spans="1:9" ht="13.5" thickBot="1">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="38"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="35"/>
     </row>
     <row r="37" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="38" spans="1:9" ht="13.5" thickBot="1">
       <c r="A38" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="35"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" ht="13.5" thickBot="1">
       <c r="A39" s="11"/>
@@ -2320,27 +2475,27 @@
       <c r="A40" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="35"/>
     </row>
     <row r="41" spans="1:9" ht="13.5" thickBot="1">
       <c r="A41" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="35"/>
     </row>
     <row r="42" spans="1:9">
       <c r="B42" s="12"/>
@@ -2357,16 +2512,16 @@
       <c r="A44" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="35"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="38"/>
     </row>
     <row r="45" spans="1:9" ht="13.5" thickBot="1">
       <c r="A45" s="11"/>
@@ -2399,27 +2554,27 @@
       <c r="A46" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="38"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="35"/>
     </row>
     <row r="47" spans="1:9" ht="13.5" thickBot="1">
       <c r="A47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="35"/>
     </row>
     <row r="48" spans="1:9">
       <c r="B48" s="12"/>
@@ -2436,16 +2591,16 @@
       <c r="A50" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="33" t="s">
+      <c r="B50" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="35"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="38"/>
     </row>
     <row r="51" spans="1:9" ht="13.5" thickBot="1">
       <c r="A51" s="11"/>
@@ -2478,43 +2633,43 @@
       <c r="A52" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="35"/>
     </row>
     <row r="53" spans="1:9" ht="13.5" thickBot="1">
       <c r="A53" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="38"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="35"/>
     </row>
     <row r="55" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="56" spans="1:9" ht="13.5" thickBot="1">
       <c r="A56" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="35"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="38"/>
     </row>
     <row r="57" spans="1:9" ht="13.5" thickBot="1">
       <c r="A57" s="11"/>
@@ -2547,43 +2702,43 @@
       <c r="A58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="38"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="35"/>
     </row>
     <row r="59" spans="1:9" ht="13.5" thickBot="1">
       <c r="A59" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="38"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="35"/>
     </row>
     <row r="61" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="62" spans="1:9" ht="13.5" thickBot="1">
       <c r="A62" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="35"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="38"/>
     </row>
     <row r="63" spans="1:9" ht="13.5" thickBot="1">
       <c r="A63" s="11"/>
@@ -2616,43 +2771,43 @@
       <c r="A64" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="38"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="35"/>
     </row>
     <row r="65" spans="1:9" ht="13.5" thickBot="1">
       <c r="A65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="38"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="35"/>
     </row>
     <row r="67" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="68" spans="1:9" ht="13.5" thickBot="1">
       <c r="A68" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="33" t="s">
+      <c r="B68" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="34"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="35"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="38"/>
     </row>
     <row r="69" spans="1:9" ht="13.5" thickBot="1">
       <c r="A69" s="11"/>
@@ -2685,43 +2840,43 @@
       <c r="A70" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="36"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="37"/>
-      <c r="H70" s="37"/>
-      <c r="I70" s="38"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
+      <c r="H70" s="34"/>
+      <c r="I70" s="35"/>
     </row>
     <row r="71" spans="1:9" ht="13.5" thickBot="1">
       <c r="A71" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="36"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="38"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="34"/>
+      <c r="H71" s="34"/>
+      <c r="I71" s="35"/>
     </row>
     <row r="73" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="74" spans="1:9" ht="13.5" thickBot="1">
       <c r="A74" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="33" t="s">
+      <c r="B74" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="35"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="38"/>
     </row>
     <row r="75" spans="1:9" ht="13.5" thickBot="1">
       <c r="A75" s="11"/>
@@ -2754,43 +2909,43 @@
       <c r="A76" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B76" s="36"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="37"/>
-      <c r="I76" s="38"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
+      <c r="H76" s="34"/>
+      <c r="I76" s="35"/>
     </row>
     <row r="77" spans="1:9" ht="13.5" thickBot="1">
       <c r="A77" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="36"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="37"/>
-      <c r="I77" s="38"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="34"/>
+      <c r="G77" s="34"/>
+      <c r="H77" s="34"/>
+      <c r="I77" s="35"/>
     </row>
     <row r="79" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="80" spans="1:9" ht="13.5" thickBot="1">
       <c r="A80" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B80" s="33" t="s">
+      <c r="B80" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="34"/>
-      <c r="H80" s="34"/>
-      <c r="I80" s="35"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="38"/>
     </row>
     <row r="81" spans="1:9" ht="13.5" thickBot="1">
       <c r="A81" s="11"/>
@@ -2823,40 +2978,46 @@
       <c r="A82" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B82" s="36"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="37"/>
-      <c r="H82" s="37"/>
-      <c r="I82" s="38"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="34"/>
+      <c r="H82" s="34"/>
+      <c r="I82" s="35"/>
     </row>
     <row r="83" spans="1:9" ht="13.5" thickBot="1">
       <c r="A83" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="36"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="37"/>
-      <c r="I83" s="38"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="34"/>
+      <c r="G83" s="34"/>
+      <c r="H83" s="34"/>
+      <c r="I83" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B68:I68"/>
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B77:I77"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B71:I71"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B62:I62"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B59:I59"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
@@ -2873,22 +3034,16 @@
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B62:I62"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B59:I59"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="B70:I70"/>
+    <mergeCell ref="B68:I68"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B77:I77"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="B71:I71"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>